<commit_message>
Replace the position of the variable STATIC_EXTRACTORS in the api.py file
</commit_message>
<xml_diff>
--- a/bank/bukti_matching/bca_matching.xlsx
+++ b/bank/bukti_matching/bca_matching.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,7 +502,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45535</v>
+        <v>45657</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -516,11 +516,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>160.416.662,31</t>
+          <t>318.599.650,03</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45535</v>
+        <v>45657</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -534,7 +534,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>160.416.662,31</t>
+          <t>318.599.650,03</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -556,11 +556,11 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45536</v>
+        <v>45658</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6.574.186,00</t>
+          <t>13.483.175,00</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -570,11 +570,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>166.990.848,31</t>
+          <t>332.082.825,03</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45536</v>
+        <v>45658</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -583,12 +583,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>6.574.186,00</t>
+          <t>13.483.175,00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>166.990.848,31</t>
+          <t>332.082.825,03</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -614,11 +614,11 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45537</v>
+        <v>45659</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4.151.852,00</t>
+          <t>6.525.848,00</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -628,11 +628,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>171.142.700,31</t>
+          <t>338.608.673,03</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45537</v>
+        <v>45659</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -641,12 +641,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4.151.852,00</t>
+          <t>6.525.848,00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>171.142.700,31</t>
+          <t>338.608.673,03</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -672,39 +672,39 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45538</v>
+        <v>45659</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2.606.550,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>27.050.000,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>173.749.250,31</t>
+          <t>311.558.673,03</t>
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>45538</v>
+        <v>45659</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>27.050.000,00</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2.606.550,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>173.749.250,31</t>
+          <t>311.558.673,03</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -730,11 +730,11 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45539</v>
+        <v>45660</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>972.180,00</t>
+          <t>33.265.241,00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -744,11 +744,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>174.721.430,31</t>
+          <t>344.823.914,03</t>
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45539</v>
+        <v>45660</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -757,12 +757,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>972.180,00</t>
+          <t>33.265.241,00</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>174.721.430,31</t>
+          <t>344.823.914,03</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -788,11 +788,11 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45540</v>
+        <v>45661</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>577.416,00</t>
+          <t>9.423.862,00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -802,11 +802,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>175.298.846,31</t>
+          <t>354.247.776,03</t>
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>45540</v>
+        <v>45661</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -815,12 +815,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>577.416,00</t>
+          <t>9.423.862,00</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>175.298.846,31</t>
+          <t>354.247.776,03</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -846,11 +846,11 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45544</v>
+        <v>45662</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>12.239.381,00</t>
+          <t>8.572.629,00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -860,11 +860,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>187.538.227,31</t>
+          <t>362.820.405,03</t>
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>45544</v>
+        <v>45662</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -873,12 +873,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>12.239.381,00</t>
+          <t>8.572.629,00</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>187.538.227,31</t>
+          <t>362.820.405,03</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -904,11 +904,11 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45545</v>
+        <v>45662</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>60.988.829,00</t>
+          <t>1.023.153,12</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -918,11 +918,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>248.527.056,31</t>
+          <t>363.843.558,15</t>
         </is>
       </c>
       <c r="E9" s="2" t="n">
-        <v>45545</v>
+        <v>45662</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -931,12 +931,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>60.988.829,00</t>
+          <t>1.023.153,12</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>248.527.056,31</t>
+          <t>363.843.558,15</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -962,39 +962,39 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45545</v>
+        <v>45663</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>8.164.244,00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>58.025.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>190.502.056,31</t>
+          <t>372.007.802,15</t>
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>45545</v>
+        <v>45663</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>58.025.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>8.164.244,00</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>190.502.056,31</t>
+          <t>372.007.802,15</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1020,39 +1020,39 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45545</v>
+        <v>45664</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>7.306.984,00</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>54.405.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>136.097.056,31</t>
+          <t>379.314.786,15</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>45545</v>
+        <v>45664</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>54.405.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>7.306.984,00</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>136.097.056,31</t>
+          <t>379.314.786,15</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1078,11 +1078,11 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45546</v>
+        <v>45664</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11.680.239,00</t>
+          <t>6.121.898,00</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1092,10 +1092,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>147.777.295,31</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
+          <t>385.436.684,15</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>45664</v>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>0,00</t>
@@ -1103,17 +1105,17 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>6.121.898,00</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>136.097.056,31</t>
+          <t>385.436.684,15</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>11.680.239,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1123,7 +1125,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Unmatched</t>
+          <t>Matched</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1134,11 +1136,11 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45547</v>
+        <v>45665</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>12.405.939,00</t>
+          <t>5.570.888,00</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1148,11 +1150,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>160.183.234,31</t>
+          <t>391.007.572,15</t>
         </is>
       </c>
       <c r="E13" s="2" t="n">
-        <v>45547</v>
+        <v>45665</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1161,12 +1163,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>12.405.939,00</t>
+          <t>5.570.888,00</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>148.502.995,31</t>
+          <t>391.007.572,15</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1192,39 +1194,39 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45547</v>
+        <v>45666</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>4.360.016,00</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>12.000.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>148.183.234,31</t>
+          <t>395.367.588,15</t>
         </is>
       </c>
       <c r="E14" s="2" t="n">
-        <v>45547</v>
+        <v>45666</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>12.000.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>4.360.016,00</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>136.502.995,31</t>
+          <t>395.367.588,15</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1250,39 +1252,39 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45548</v>
+        <v>45666</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>805.240,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>244.730.000,00</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>148.988.474,31</t>
+          <t>150.637.588,15</t>
         </is>
       </c>
       <c r="E15" s="2" t="n">
-        <v>45548</v>
+        <v>45666</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>244.730.000,00</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>805.240,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>137.308.235,31</t>
+          <t>150.637.588,15</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1308,11 +1310,11 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45549</v>
+        <v>45667</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>9.705.970,00</t>
+          <t>9.181.621,00</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1322,11 +1324,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>158.694.444,31</t>
+          <t>159.819.209,15</t>
         </is>
       </c>
       <c r="E16" s="2" t="n">
-        <v>45549</v>
+        <v>45667</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1335,12 +1337,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>9.705.970,00</t>
+          <t>9.181.621,00</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>147.014.205,31</t>
+          <t>159.819.209,15</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1366,11 +1368,11 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45550</v>
+        <v>45668</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>3.442.950,00</t>
+          <t>20.261.504,00</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1380,11 +1382,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>162.137.394,31</t>
+          <t>180.080.713,15</t>
         </is>
       </c>
       <c r="E17" s="2" t="n">
-        <v>45550</v>
+        <v>45668</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1393,12 +1395,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>3.442.950,00</t>
+          <t>20.261.504,00</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>150.457.155,31</t>
+          <t>180.080.713,15</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1424,11 +1426,11 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45551</v>
+        <v>45669</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>6.152.053,00</t>
+          <t>10.643.898,00</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1438,11 +1440,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>168.289.447,31</t>
+          <t>190.724.611,15</t>
         </is>
       </c>
       <c r="E18" s="2" t="n">
-        <v>45551</v>
+        <v>45669</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1451,12 +1453,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>6.152.053,00</t>
+          <t>10.643.898,00</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>156.609.208,31</t>
+          <t>190.724.611,15</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1482,11 +1484,11 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45552</v>
+        <v>45670</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>12.834.834,00</t>
+          <t>11.136.960,00</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1496,11 +1498,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>181.124.281,31</t>
+          <t>201.861.571,15</t>
         </is>
       </c>
       <c r="E19" s="2" t="n">
-        <v>45552</v>
+        <v>45670</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1509,12 +1511,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>12.834.834,00</t>
+          <t>11.136.960,00</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>169.444.042,31</t>
+          <t>201.861.571,15</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1540,11 +1542,11 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45553</v>
+        <v>45671</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>10.119.323,00</t>
+          <t>2.628.790,00</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1554,11 +1556,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>191.243.604,31</t>
+          <t>204.490.361,15</t>
         </is>
       </c>
       <c r="E20" s="2" t="n">
-        <v>45553</v>
+        <v>45671</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1567,12 +1569,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>10.119.323,00</t>
+          <t>2.628.790,00</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>179.563.365,31</t>
+          <t>204.490.361,15</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1598,7 +1600,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45553</v>
+        <v>45671</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1607,20 +1609,20 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>4.910.000,00</t>
+          <t>35.550.000,00</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>186.333.604,31</t>
+          <t>168.940.361,15</t>
         </is>
       </c>
       <c r="E21" s="2" t="n">
-        <v>45553</v>
+        <v>45671</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>4.910.000,00</t>
+          <t>35.550.000,00</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1630,7 +1632,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>174.653.365,31</t>
+          <t>168.940.361,15</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1656,11 +1658,11 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45554</v>
+        <v>45672</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3.018.943,00</t>
+          <t>6.875.000,00</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1670,11 +1672,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>189.352.547,31</t>
+          <t>175.815.361,15</t>
         </is>
       </c>
       <c r="E22" s="2" t="n">
-        <v>45554</v>
+        <v>45672</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1683,12 +1685,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>3.018.943,00</t>
+          <t>6.875.000,00</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>177.672.308,31</t>
+          <t>175.815.361,15</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1714,11 +1716,11 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45555</v>
+        <v>45672</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1.380.741,00</t>
+          <t>5.139.229,00</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1728,11 +1730,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>190.733.288,31</t>
+          <t>180.954.590,15</t>
         </is>
       </c>
       <c r="E23" s="2" t="n">
-        <v>45555</v>
+        <v>45672</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1741,12 +1743,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>1.380.741,00</t>
+          <t>5.139.229,00</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>179.053.049,31</t>
+          <t>180.954.590,15</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1772,39 +1774,39 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45555</v>
+        <v>45673</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>7.728.376,00</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>20.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>190.713.288,31</t>
+          <t>188.682.966,15</t>
         </is>
       </c>
       <c r="E24" s="2" t="n">
-        <v>45555</v>
+        <v>45673</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>20.000,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>7.728.376,00</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>179.033.049,31</t>
+          <t>188.682.966,15</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1830,11 +1832,11 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45556</v>
+        <v>45674</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1.865.800,00</t>
+          <t>6.895.087,00</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1844,11 +1846,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>192.579.088,31</t>
+          <t>195.578.053,15</t>
         </is>
       </c>
       <c r="E25" s="2" t="n">
-        <v>45556</v>
+        <v>45674</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1857,12 +1859,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1.865.800,00</t>
+          <t>6.895.087,00</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>180.898.849,31</t>
+          <t>195.578.053,15</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1888,39 +1890,39 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45557</v>
+        <v>45674</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>6.848.379,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>20.000,00</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>199.427.467,31</t>
+          <t>195.558.053,15</t>
         </is>
       </c>
       <c r="E26" s="2" t="n">
-        <v>45557</v>
+        <v>45674</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>20.000,00</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>6.848.379,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>187.747.228,31</t>
+          <t>195.558.053,15</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1946,11 +1948,11 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45558</v>
+        <v>45675</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>8.410.830,00</t>
+          <t>8.014.683,00</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1960,11 +1962,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>207.838.297,31</t>
+          <t>203.572.736,15</t>
         </is>
       </c>
       <c r="E27" s="2" t="n">
-        <v>45558</v>
+        <v>45675</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1973,12 +1975,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>8.410.830,00</t>
+          <t>8.014.683,00</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>196.158.058,31</t>
+          <t>203.572.736,15</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -2004,11 +2006,11 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45559</v>
+        <v>45676</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3.972.041,00</t>
+          <t>6.255.144,00</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2018,11 +2020,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>211.810.338,31</t>
+          <t>209.827.880,15</t>
         </is>
       </c>
       <c r="E28" s="2" t="n">
-        <v>45559</v>
+        <v>45676</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -2031,12 +2033,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>3.972.041,00</t>
+          <t>6.255.144,00</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>200.130.099,31</t>
+          <t>209.827.880,15</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2062,11 +2064,11 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45560</v>
+        <v>45677</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>13.889.072,00</t>
+          <t>10.723.347,00</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2076,11 +2078,11 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>225.699.410,31</t>
+          <t>220.551.227,15</t>
         </is>
       </c>
       <c r="E29" s="2" t="n">
-        <v>45560</v>
+        <v>45677</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -2089,12 +2091,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>13.889.072,00</t>
+          <t>10.723.347,00</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>214.019.171,31</t>
+          <t>220.551.227,15</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2120,11 +2122,11 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45561</v>
+        <v>45678</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>6.178.795,00</t>
+          <t>2.563.183,00</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2134,11 +2136,11 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>231.878.205,31</t>
+          <t>223.114.410,15</t>
         </is>
       </c>
       <c r="E30" s="2" t="n">
-        <v>45561</v>
+        <v>45678</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -2147,12 +2149,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>6.178.795,00</t>
+          <t>2.563.183,00</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>220.197.966,31</t>
+          <t>223.114.410,15</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2178,11 +2180,11 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45562</v>
+        <v>45679</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1.805.319,00</t>
+          <t>17.828.643,00</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2192,11 +2194,11 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>233.683.524,31</t>
+          <t>240.943.053,15</t>
         </is>
       </c>
       <c r="E31" s="2" t="n">
-        <v>45562</v>
+        <v>45679</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -2205,12 +2207,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>1.805.319,00</t>
+          <t>17.828.643,00</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>222.003.285,31</t>
+          <t>240.943.053,15</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2236,39 +2238,39 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45563</v>
+        <v>45679</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>533.624,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>11.125.000,00</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>234.217.148,31</t>
+          <t>229.818.053,15</t>
         </is>
       </c>
       <c r="E32" s="2" t="n">
-        <v>45563</v>
+        <v>45679</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>11.125.000,00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>533.624,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>222.536.909,31</t>
+          <t>229.818.053,15</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2294,11 +2296,11 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45564</v>
+        <v>45680</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>12.537.751,00</t>
+          <t>925.000,00</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2308,11 +2310,11 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>246.754.899,31</t>
+          <t>230.743.053,15</t>
         </is>
       </c>
       <c r="E33" s="2" t="n">
-        <v>45564</v>
+        <v>45678</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -2321,12 +2323,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>12.537.751,00</t>
+          <t>925.000,00</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>235.074.660,31</t>
+          <t>230.743.053,15</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -2352,11 +2354,11 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45565</v>
+        <v>45680</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>15.024.496,00</t>
+          <t>4.094.940,00</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2366,11 +2368,11 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>261.779.395,31</t>
+          <t>234.837.993,15</t>
         </is>
       </c>
       <c r="E34" s="2" t="n">
-        <v>45565</v>
+        <v>45680</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -2379,12 +2381,12 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>15.024.496,00</t>
+          <t>4.094.940,00</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>250.099.156,31</t>
+          <t>234.837.993,15</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -2410,11 +2412,11 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45565</v>
+        <v>45681</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1.540,50</t>
+          <t>4.968.134,00</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2424,11 +2426,11 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>261.780.935,81</t>
+          <t>239.806.127,15</t>
         </is>
       </c>
       <c r="E35" s="2" t="n">
-        <v>45565</v>
+        <v>45681</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -2437,12 +2439,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>1.540,50</t>
+          <t>4.968.134,00</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>250.100.696,81</t>
+          <t>239.806.127,15</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2468,39 +2470,39 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45565</v>
+        <v>45682</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>7.988.959,00</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>308,10</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>261.780.627,71</t>
+          <t>247.795.086,15</t>
         </is>
       </c>
       <c r="E36" s="2" t="n">
-        <v>45565</v>
+        <v>45682</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>308,10</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>0,00</t>
+          <t>7.988.959,00</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>250.100.388,71</t>
+          <t>247.795.086,15</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2526,44 +2528,44 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45565</v>
+        <v>45683</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>230.724.273,50</t>
+          <t>8.718.225,00</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>129.360.308,10</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>261.780.627,71</t>
+          <t>256.513.311,15</t>
         </is>
       </c>
       <c r="E37" s="2" t="n">
-        <v>45565</v>
+        <v>45683</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>129.360.308,10</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>219.044.034,50</t>
+          <t>8.718.225,00</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>250.100.388,71</t>
+          <t>256.513.311,15</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>11.680.239,00</t>
+          <t>0,00</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2573,10 +2575,532 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
+          <t>Matched</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>45684</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>14.955.267,00</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>271.468.578,15</t>
+        </is>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>45684</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>14.955.267,00</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>271.468.578,15</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>8.589.883,00</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>280.058.461,15</t>
+        </is>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>45685</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>8.589.883,00</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>280.058.461,15</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2.772.665,00</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>282.831.126,15</t>
+        </is>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2.772.665,00</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>282.831.126,15</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>66.415.000,00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>216.416.126,15</t>
+        </is>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>45686</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>66.415.000,00</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>216.416.126,15</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45687</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>1.767.600,00</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>218.183.726,15</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>45687</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>1.767.600,00</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>218.183.726,15</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>45688</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>5.317.589,00</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>223.501.315,15</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>45688</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>5.317.589,00</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>223.501.315,15</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>45688</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2.125,07</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>223.503.440,22</t>
+        </is>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>45688</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2.125,07</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>223.503.440,22</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45688</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>425,01</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>223.503.015,21</t>
+        </is>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>45688</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>425,01</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>223.503.015,21</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Matched</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>45688</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>289.793.790,19</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>384.890.425,01</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>223.503.015,21</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>45688</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>384.890.425,01</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>289.793.790,19</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>223.503.015,21</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
           <t>Closing Balance</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2631,16 +3155,16 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45535</v>
+        <v>45657</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>160.416.662,31</t>
+          <t>318.599.650,03</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>160.416.662,31</t>
+          <t>318.599.650,03</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2656,21 +3180,21 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45565</v>
+        <v>45688</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>261.780.627,71</t>
+          <t>223.503.015,21</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>250.100.388,71</t>
+          <t>223.503.015,21</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>11.680.239,00</t>
+          <t>0,00</t>
         </is>
       </c>
     </row>

</xml_diff>